<commit_message>
Se separa version para b05s100 y b05s111
</commit_message>
<xml_diff>
--- a/Historial/interpolacion.xlsx
+++ b/Historial/interpolacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="15" windowWidth="8115" windowHeight="3165"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="8115" windowHeight="3180"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -144,56 +144,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="3"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -504,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>11</v>
@@ -540,22 +495,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>6</v>
+        <v>595</v>
       </c>
       <c r="F3" s="7">
         <v>200</v>
       </c>
       <c r="G3" s="5">
         <f>FORECAST(F3,$C$2:$C$3,$C$4:$C$5)</f>
-        <v>-4.4408920985006262E-16</v>
+        <v>-5.4812834224598532</v>
       </c>
       <c r="H3" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F3-C$4)+C$2)/C$9)</f>
-        <v>0</v>
+        <f t="shared" ref="H3:H12" si="0">TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F3-C$4)+C$2)/C$9)</f>
+        <v>-9</v>
       </c>
       <c r="I3" s="5">
         <f>ABS(G3-H3)</f>
-        <v>4.4408920985006262E-16</v>
+        <v>3.5187165775401468</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -563,22 +518,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="F4" s="7">
         <v>230</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" ref="G4:G25" si="0">FORECAST(F4,$C$2:$C$3,$C$4:$C$5)</f>
-        <v>0.32142857142857117</v>
+        <f t="shared" ref="G4:G25" si="1">FORECAST(F4,$C$2:$C$3,$C$4:$C$5)</f>
+        <v>26.122994652406476</v>
       </c>
       <c r="H4" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F4-C$4)+C$2)/C$9)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" ref="I4:I12" si="1">ABS(G4-H4)</f>
-        <v>0.32142857142857117</v>
+        <f t="shared" ref="I4:I12" si="2">ABS(G4-H4)</f>
+        <v>4.1229946524064758</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -586,22 +541,22 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>760</v>
+        <v>770</v>
       </c>
       <c r="F5" s="7">
         <v>260</v>
       </c>
       <c r="G5" s="5">
+        <f t="shared" si="1"/>
+        <v>57.727272727272748</v>
+      </c>
+      <c r="H5" s="5">
         <f t="shared" si="0"/>
-        <v>0.64285714285714235</v>
-      </c>
-      <c r="H5" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F5-C$4)+C$2)/C$9)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I5" s="5">
-        <f t="shared" si="1"/>
-        <v>0.64285714285714235</v>
+        <f t="shared" si="2"/>
+        <v>4.7272727272727479</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -610,16 +565,16 @@
         <v>290</v>
       </c>
       <c r="G6" s="5">
+        <f t="shared" si="1"/>
+        <v>89.331550802139077</v>
+      </c>
+      <c r="H6" s="5">
         <f t="shared" si="0"/>
-        <v>0.96428571428571397</v>
-      </c>
-      <c r="H6" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F6-C$4)+C$2)/C$9)</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I6" s="5">
-        <f t="shared" si="1"/>
-        <v>0.96428571428571397</v>
+        <f t="shared" si="2"/>
+        <v>4.3315508021390769</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -627,22 +582,22 @@
         <v>11</v>
       </c>
       <c r="C7" s="1">
-        <v>3650</v>
+        <v>803</v>
       </c>
       <c r="F7" s="7">
         <v>320</v>
       </c>
       <c r="G7" s="5">
+        <f t="shared" si="1"/>
+        <v>120.93582887700541</v>
+      </c>
+      <c r="H7" s="5">
         <f t="shared" si="0"/>
-        <v>1.2857142857142856</v>
-      </c>
-      <c r="H7" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F7-C$4)+C$2)/C$9)</f>
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="I7" s="5">
-        <f t="shared" si="1"/>
-        <v>0.28571428571428559</v>
+        <f t="shared" si="2"/>
+        <v>4.935828877005406</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -650,16 +605,16 @@
         <v>350</v>
       </c>
       <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>152.54010695187168</v>
+      </c>
+      <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>1.6071428571428568</v>
-      </c>
-      <c r="H8" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F8-C$4)+C$2)/C$9)</f>
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" si="1"/>
-        <v>0.60714285714285676</v>
+        <f t="shared" si="2"/>
+        <v>4.5401069518716781</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -673,16 +628,16 @@
         <v>380</v>
       </c>
       <c r="G9" s="5">
+        <f t="shared" si="1"/>
+        <v>184.14438502673801</v>
+      </c>
+      <c r="H9" s="5">
         <f t="shared" si="0"/>
-        <v>1.9285714285714279</v>
-      </c>
-      <c r="H9" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F9-C$4)+C$2)/C$9)</f>
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="I9" s="5">
-        <f t="shared" si="1"/>
-        <v>0.92857142857142794</v>
+        <f t="shared" si="2"/>
+        <v>4.1443850267380071</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -690,16 +645,16 @@
         <v>410</v>
       </c>
       <c r="G10" s="5">
+        <f t="shared" si="1"/>
+        <v>215.74866310160434</v>
+      </c>
+      <c r="H10" s="5">
         <f t="shared" si="0"/>
-        <v>2.25</v>
-      </c>
-      <c r="H10" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F10-C$4)+C$2)/C$9)</f>
-        <v>2</v>
+        <v>211</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
+        <f t="shared" si="2"/>
+        <v>4.7486631016043361</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -708,30 +663,30 @@
       </c>
       <c r="B11">
         <f>C3</f>
-        <v>6</v>
+        <v>595</v>
       </c>
       <c r="C11">
         <f>C2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f>B11-C11</f>
-        <v>6</v>
+        <v>591</v>
       </c>
       <c r="F11" s="7">
         <v>440</v>
       </c>
       <c r="G11" s="5">
+        <f t="shared" si="1"/>
+        <v>247.35294117647061</v>
+      </c>
+      <c r="H11" s="5">
         <f t="shared" si="0"/>
-        <v>2.5714285714285712</v>
-      </c>
-      <c r="H11" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F11-C$4)+C$2)/C$9)</f>
-        <v>2</v>
+        <v>243</v>
       </c>
       <c r="I11" s="5">
-        <f t="shared" si="1"/>
-        <v>0.57142857142857117</v>
+        <f t="shared" si="2"/>
+        <v>4.3529411764706083</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -740,30 +695,30 @@
       </c>
       <c r="B12">
         <f>C5</f>
-        <v>760</v>
+        <v>770</v>
       </c>
       <c r="C12">
         <f>C4</f>
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D12">
         <f>B12-C12</f>
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F12" s="7">
         <v>470</v>
       </c>
       <c r="G12" s="5">
+        <f t="shared" si="1"/>
+        <v>278.95721925133694</v>
+      </c>
+      <c r="H12" s="5">
         <f t="shared" si="0"/>
-        <v>2.8928571428571423</v>
-      </c>
-      <c r="H12" s="5">
-        <f>TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F12-C$4)+C$2)/C$9)</f>
-        <v>2</v>
+        <v>274</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="1"/>
-        <v>0.89285714285714235</v>
+        <f t="shared" si="2"/>
+        <v>4.9572192513369373</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -772,7 +727,7 @@
       </c>
       <c r="B13">
         <f>D11</f>
-        <v>6</v>
+        <v>591</v>
       </c>
       <c r="C13">
         <f>C9</f>
@@ -780,22 +735,22 @@
       </c>
       <c r="D13">
         <f>B13*C13</f>
-        <v>60000</v>
+        <v>5910000</v>
       </c>
       <c r="F13" s="7">
         <v>500</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="0"/>
-        <v>3.2142857142857135</v>
+        <f t="shared" si="1"/>
+        <v>310.56149732620327</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" ref="H13:H25" si="2">TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F13-C$4)+C$2)/C$9)</f>
-        <v>3</v>
+        <f t="shared" ref="H13:H25" si="3">TRUNC((TRUNC(((C$3-C$2)*C$9)/(C$5-C$4))*(F13-C$4)+C$2)/C$9)</f>
+        <v>306</v>
       </c>
       <c r="I13" s="5">
-        <f t="shared" ref="I13:I25" si="3">ABS(G13-H13)</f>
-        <v>0.21428571428571352</v>
+        <f t="shared" ref="I13:I25" si="4">ABS(G13-H13)</f>
+        <v>4.5614973262032663</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -804,30 +759,30 @@
       </c>
       <c r="B14">
         <f>D13</f>
-        <v>60000</v>
+        <v>5910000</v>
       </c>
       <c r="C14">
         <f>D12</f>
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D14">
         <f>TRUNC(B14/C14)</f>
-        <v>107</v>
+        <v>10534</v>
       </c>
       <c r="F14" s="7">
         <v>530</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="0"/>
-        <v>3.5357142857142856</v>
+        <f t="shared" si="1"/>
+        <v>342.1657754010696</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>338</v>
       </c>
       <c r="I14" s="5">
-        <f t="shared" si="3"/>
-        <v>0.53571428571428559</v>
+        <f t="shared" si="4"/>
+        <v>4.1657754010695953</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -836,30 +791,30 @@
       </c>
       <c r="B15">
         <f>C7</f>
-        <v>3650</v>
+        <v>803</v>
       </c>
       <c r="C15">
         <f>C4</f>
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D15">
         <f>B15-C15</f>
-        <v>3450</v>
+        <v>594</v>
       </c>
       <c r="F15" s="7">
         <v>560</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="0"/>
-        <v>3.8571428571428568</v>
+        <f t="shared" si="1"/>
+        <v>373.77005347593592</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>369</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="3"/>
-        <v>0.85714285714285676</v>
+        <f t="shared" si="4"/>
+        <v>4.7700534759359243</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -868,94 +823,94 @@
       </c>
       <c r="B16">
         <f>D14</f>
-        <v>107</v>
+        <v>10534</v>
       </c>
       <c r="C16">
         <f>D15</f>
-        <v>3450</v>
+        <v>594</v>
       </c>
       <c r="D16">
         <f>B16*C16</f>
-        <v>369150</v>
+        <v>6257196</v>
       </c>
       <c r="F16" s="7">
         <v>590</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="0"/>
-        <v>4.1785714285714279</v>
+        <f t="shared" si="1"/>
+        <v>405.37433155080214</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>401</v>
       </c>
       <c r="I16" s="5">
-        <f t="shared" si="3"/>
-        <v>0.17857142857142794</v>
+        <f t="shared" si="4"/>
+        <v>4.3743315508021396</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <f>D16</f>
-        <v>369150</v>
+        <v>6257196</v>
       </c>
       <c r="C17">
-        <f>C2</f>
-        <v>0</v>
+        <f>C9</f>
+        <v>10000</v>
       </c>
       <c r="D17">
-        <f>B17+C17</f>
-        <v>369150</v>
+        <f>TRUNC(B17/C17)</f>
+        <v>625</v>
       </c>
       <c r="F17" s="7">
         <v>620</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
+        <f t="shared" si="1"/>
+        <v>436.97860962566847</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>432</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
+        <f t="shared" si="4"/>
+        <v>4.9786096256684687</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <f>D17</f>
-        <v>369150</v>
+        <v>625</v>
       </c>
       <c r="C18">
-        <f>C9</f>
-        <v>10000</v>
+        <f>C2</f>
+        <v>4</v>
       </c>
       <c r="D18">
-        <f>TRUNC(B18/C18)</f>
-        <v>36</v>
+        <f>B18+C18</f>
+        <v>629</v>
       </c>
       <c r="F18" s="7">
         <v>650</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="0"/>
-        <v>4.8214285714285712</v>
+        <f t="shared" si="1"/>
+        <v>468.5828877005348</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>464</v>
       </c>
       <c r="I18" s="5">
-        <f t="shared" si="3"/>
-        <v>0.82142857142857117</v>
+        <f t="shared" si="4"/>
+        <v>4.5828877005347977</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -963,16 +918,16 @@
         <v>680</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="0"/>
-        <v>5.1428571428571423</v>
+        <f t="shared" si="1"/>
+        <v>500.18716577540113</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>496</v>
       </c>
       <c r="I19" s="5">
-        <f t="shared" si="3"/>
-        <v>0.14285714285714235</v>
+        <f t="shared" si="4"/>
+        <v>4.1871657754011267</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -981,22 +936,22 @@
       </c>
       <c r="C20" s="3">
         <f>FORECAST(C7,C2:C3,C4:C5)</f>
-        <v>36.964285714285708</v>
+        <v>629.76470588235293</v>
       </c>
       <c r="F20" s="7">
         <v>710</v>
       </c>
       <c r="G20" s="5">
-        <f t="shared" si="0"/>
-        <v>5.4642857142857144</v>
+        <f t="shared" si="1"/>
+        <v>531.79144385026746</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>527</v>
       </c>
       <c r="I20" s="5">
-        <f t="shared" si="3"/>
-        <v>0.46428571428571441</v>
+        <f t="shared" si="4"/>
+        <v>4.7914438502674557</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1005,22 +960,22 @@
       </c>
       <c r="C21" s="2">
         <f>D18</f>
-        <v>36</v>
+        <v>629</v>
       </c>
       <c r="F21" s="7">
         <v>740</v>
       </c>
       <c r="G21" s="5">
-        <f t="shared" si="0"/>
-        <v>5.7857142857142856</v>
+        <f t="shared" si="1"/>
+        <v>563.39572192513378</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>559</v>
       </c>
       <c r="I21" s="5">
-        <f t="shared" si="3"/>
-        <v>0.78571428571428559</v>
+        <f t="shared" si="4"/>
+        <v>4.3957219251337847</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1028,16 +983,16 @@
         <v>770</v>
       </c>
       <c r="G22" s="5">
-        <f t="shared" si="0"/>
-        <v>6.1071428571428568</v>
+        <f t="shared" si="1"/>
+        <v>595</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>590</v>
       </c>
       <c r="I22" s="5">
-        <f t="shared" si="3"/>
-        <v>0.10714285714285676</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1045,16 +1000,16 @@
         <v>800</v>
       </c>
       <c r="G23" s="5">
-        <f t="shared" si="0"/>
-        <v>6.4285714285714279</v>
+        <f t="shared" si="1"/>
+        <v>626.60427807486633</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>622</v>
       </c>
       <c r="I23" s="5">
-        <f t="shared" si="3"/>
-        <v>0.42857142857142794</v>
+        <f t="shared" si="4"/>
+        <v>4.604278074866329</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1062,16 +1017,16 @@
         <v>830</v>
       </c>
       <c r="G24" s="5">
-        <f t="shared" si="0"/>
-        <v>6.7499999999999991</v>
+        <f t="shared" si="1"/>
+        <v>658.20855614973266</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>654</v>
       </c>
       <c r="I24" s="5">
-        <f t="shared" si="3"/>
-        <v>0.74999999999999911</v>
+        <f t="shared" si="4"/>
+        <v>4.208556149732658</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1079,24 +1034,24 @@
         <v>860</v>
       </c>
       <c r="G25" s="5">
-        <f t="shared" si="0"/>
-        <v>7.0714285714285703</v>
+        <f t="shared" si="1"/>
+        <v>689.81283422459899</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <f t="shared" si="3"/>
+        <v>685</v>
       </c>
       <c r="I25" s="5">
-        <f t="shared" si="3"/>
-        <v>7.1428571428570287E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.812834224598987</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:D18">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>4294967295</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>65535</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>